<commit_message>
file reclami implementato e pulito
</commit_message>
<xml_diff>
--- a/reclami.xlsx
+++ b/reclami.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/424ae4c6f4efc74d/Desktop/Workspace/capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FEE507CB-13F9-494B-94E1-D27C6FEC134D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E79BDA64-A457-4705-862D-D6B7DCD9616F}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{FEE507CB-13F9-494B-94E1-D27C6FEC134D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F19CAD8-07D5-48DE-8DC5-FCCD9798F70F}"/>
   <bookViews>
-    <workbookView xWindow="25995" yWindow="-13470" windowWidth="24630" windowHeight="11865" xr2:uid="{B49F0930-AF17-BA40-A0CD-03D467FE61F3}"/>
+    <workbookView xWindow="2970" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B49F0930-AF17-BA40-A0CD-03D467FE61F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2075" uniqueCount="787">
   <si>
     <t>PM14</t>
   </si>
@@ -1988,6 +1988,540 @@
   </si>
   <si>
     <t>46.0049918593186, 12.03111508125752</t>
+  </si>
+  <si>
+    <t>PM100</t>
+  </si>
+  <si>
+    <t>tegole_tesi_12_francia</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>PM101</t>
+  </si>
+  <si>
+    <t>N35</t>
+  </si>
+  <si>
+    <t>PM102</t>
+  </si>
+  <si>
+    <t>tesi_rossa</t>
+  </si>
+  <si>
+    <t>PM103</t>
+  </si>
+  <si>
+    <t>PM104</t>
+  </si>
+  <si>
+    <t>tegole_tesi_chiare</t>
+  </si>
+  <si>
+    <t>PM105</t>
+  </si>
+  <si>
+    <t>PM106</t>
+  </si>
+  <si>
+    <t>PM107</t>
+  </si>
+  <si>
+    <t>IM4B6</t>
+  </si>
+  <si>
+    <t>PM108</t>
+  </si>
+  <si>
+    <t>tesi_winter_serenissima</t>
+  </si>
+  <si>
+    <t>PM109</t>
+  </si>
+  <si>
+    <t>unicoppo_rosso_extra_12_mq</t>
+  </si>
+  <si>
+    <t>PM110</t>
+  </si>
+  <si>
+    <t>PM111</t>
+  </si>
+  <si>
+    <t>maxima_serenissima</t>
+  </si>
+  <si>
+    <t>PM112</t>
+  </si>
+  <si>
+    <t>PM113</t>
+  </si>
+  <si>
+    <t>PM114</t>
+  </si>
+  <si>
+    <t>PM115</t>
+  </si>
+  <si>
+    <t>PM116</t>
+  </si>
+  <si>
+    <t>PM117</t>
+  </si>
+  <si>
+    <t>PM118</t>
+  </si>
+  <si>
+    <t>PM119</t>
+  </si>
+  <si>
+    <t>tegole_temax_serenissima</t>
+  </si>
+  <si>
+    <t>PM120</t>
+  </si>
+  <si>
+    <t>PM121</t>
+  </si>
+  <si>
+    <t>PM122</t>
+  </si>
+  <si>
+    <t>PM123</t>
+  </si>
+  <si>
+    <t>PM124</t>
+  </si>
+  <si>
+    <t>PM125</t>
+  </si>
+  <si>
+    <t>PM126</t>
+  </si>
+  <si>
+    <t>PM127</t>
+  </si>
+  <si>
+    <t>PM128</t>
+  </si>
+  <si>
+    <t>PM129</t>
+  </si>
+  <si>
+    <t>PM130</t>
+  </si>
+  <si>
+    <t>PM131</t>
+  </si>
+  <si>
+    <t>PM132</t>
+  </si>
+  <si>
+    <t>PM133</t>
+  </si>
+  <si>
+    <t>PM134</t>
+  </si>
+  <si>
+    <t>PM135</t>
+  </si>
+  <si>
+    <t>PM136</t>
+  </si>
+  <si>
+    <t>PM137</t>
+  </si>
+  <si>
+    <t>PM138</t>
+  </si>
+  <si>
+    <t>PM139</t>
+  </si>
+  <si>
+    <t>PM140</t>
+  </si>
+  <si>
+    <t>PM141</t>
+  </si>
+  <si>
+    <t>PM142</t>
+  </si>
+  <si>
+    <t>PM143</t>
+  </si>
+  <si>
+    <t>PM144</t>
+  </si>
+  <si>
+    <t>PM145</t>
+  </si>
+  <si>
+    <t>PM146</t>
+  </si>
+  <si>
+    <t>PM147</t>
+  </si>
+  <si>
+    <t>PM148</t>
+  </si>
+  <si>
+    <t>PM149</t>
+  </si>
+  <si>
+    <t>Sfaldatura rottura aloni umiditÃ </t>
+  </si>
+  <si>
+    <t>VI80565</t>
+  </si>
+  <si>
+    <t>VI93591</t>
+  </si>
+  <si>
+    <t>VI20767</t>
+  </si>
+  <si>
+    <t>VI78375</t>
+  </si>
+  <si>
+    <t>VI82070</t>
+  </si>
+  <si>
+    <t>VI89897</t>
+  </si>
+  <si>
+    <t>VI8876</t>
+  </si>
+  <si>
+    <t>VI40320</t>
+  </si>
+  <si>
+    <t>VI61918</t>
+  </si>
+  <si>
+    <t>VI94155</t>
+  </si>
+  <si>
+    <t>VI18131</t>
+  </si>
+  <si>
+    <t>VI84886</t>
+  </si>
+  <si>
+    <t>VI25933</t>
+  </si>
+  <si>
+    <t>VI66853</t>
+  </si>
+  <si>
+    <t>VI64603</t>
+  </si>
+  <si>
+    <t>VI65119</t>
+  </si>
+  <si>
+    <t>VI9758</t>
+  </si>
+  <si>
+    <t>VI45968</t>
+  </si>
+  <si>
+    <t>VI30335</t>
+  </si>
+  <si>
+    <t>VI63302</t>
+  </si>
+  <si>
+    <t>VI74740</t>
+  </si>
+  <si>
+    <t>VI46191</t>
+  </si>
+  <si>
+    <t>VI2074</t>
+  </si>
+  <si>
+    <t>VI45630</t>
+  </si>
+  <si>
+    <t>VI31716</t>
+  </si>
+  <si>
+    <t>R210311</t>
+  </si>
+  <si>
+    <t>TRENTINOALTO_ADIGE</t>
+  </si>
+  <si>
+    <t>guaina</t>
+  </si>
+  <si>
+    <t>legno</t>
+  </si>
+  <si>
+    <t>legno_+_guaina</t>
+  </si>
+  <si>
+    <t>doppio_listello_incrociato</t>
+  </si>
+  <si>
+    <t>412.8</t>
+  </si>
+  <si>
+    <t>460.0</t>
+  </si>
+  <si>
+    <t>436.6</t>
+  </si>
+  <si>
+    <t>358.3</t>
+  </si>
+  <si>
+    <t>521.8</t>
+  </si>
+  <si>
+    <t>415.4</t>
+  </si>
+  <si>
+    <t>476.6</t>
+  </si>
+  <si>
+    <t>476.0</t>
+  </si>
+  <si>
+    <t>332.4</t>
+  </si>
+  <si>
+    <t>450.7</t>
+  </si>
+  <si>
+    <t>408.7</t>
+  </si>
+  <si>
+    <t>451.7</t>
+  </si>
+  <si>
+    <t>494.3</t>
+  </si>
+  <si>
+    <t>331.2</t>
+  </si>
+  <si>
+    <t>250.9</t>
+  </si>
+  <si>
+    <t>272.8</t>
+  </si>
+  <si>
+    <t>393.5</t>
+  </si>
+  <si>
+    <t>510.3</t>
+  </si>
+  <si>
+    <t>283.9</t>
+  </si>
+  <si>
+    <t>546.0</t>
+  </si>
+  <si>
+    <t>503.5</t>
+  </si>
+  <si>
+    <t>390.7</t>
+  </si>
+  <si>
+    <t>377.4</t>
+  </si>
+  <si>
+    <t>276.3</t>
+  </si>
+  <si>
+    <t>275.8</t>
+  </si>
+  <si>
+    <t>492.5</t>
+  </si>
+  <si>
+    <t>534.8</t>
+  </si>
+  <si>
+    <t>301.6</t>
+  </si>
+  <si>
+    <t>278.7</t>
+  </si>
+  <si>
+    <t>341.3</t>
+  </si>
+  <si>
+    <t>267.7</t>
+  </si>
+  <si>
+    <t>526.5</t>
+  </si>
+  <si>
+    <t>514.3</t>
+  </si>
+  <si>
+    <t>386.7</t>
+  </si>
+  <si>
+    <t>506.8</t>
+  </si>
+  <si>
+    <t>aperta</t>
+  </si>
+  <si>
+    <t>45.98675723232063, 11.43692728425729</t>
+  </si>
+  <si>
+    <t>45.9856883448651, 11.02872843188776</t>
+  </si>
+  <si>
+    <t>45.4516185481196, 9.92484069425045</t>
+  </si>
+  <si>
+    <t>46.04746159589854, 10.10923527942807</t>
+  </si>
+  <si>
+    <t>45.62429675866047, 11.18726614246331</t>
+  </si>
+  <si>
+    <t>45.71336625346943, 10.83253079122324</t>
+  </si>
+  <si>
+    <t>45.61627910412689, 10.13486358412795</t>
+  </si>
+  <si>
+    <t>45.82664827189913, 10.65728058409799</t>
+  </si>
+  <si>
+    <t>45.44234099501472, 11.6124859812319</t>
+  </si>
+  <si>
+    <t>45.95263277769655, 11.54157473783601</t>
+  </si>
+  <si>
+    <t>45.9381608545464, 9.76714811709203</t>
+  </si>
+  <si>
+    <t>45.51914582571865, 10.93997451735399</t>
+  </si>
+  <si>
+    <t>46.11059026862858, 10.87346928695971</t>
+  </si>
+  <si>
+    <t>46.12748075781776, 11.60706377924723</t>
+  </si>
+  <si>
+    <t>46.16037816581037, 11.216989870291</t>
+  </si>
+  <si>
+    <t>45.42627659314392, 12.43801524501797</t>
+  </si>
+  <si>
+    <t>45.44239496628192, 10.46697444705453</t>
+  </si>
+  <si>
+    <t>45.45248273186041, 12.4384098670941</t>
+  </si>
+  <si>
+    <t>46.09917227570228, 10.85865381047314</t>
+  </si>
+  <si>
+    <t>45.93129170550344, 11.95701951544305</t>
+  </si>
+  <si>
+    <t>46.05806403232562, 11.75328404314289</t>
+  </si>
+  <si>
+    <t>45.90155458938235, 10.5366242027426</t>
+  </si>
+  <si>
+    <t>45.4646739422077, 12.38432425219716</t>
+  </si>
+  <si>
+    <t>45.68043094846533, 11.56904360649918</t>
+  </si>
+  <si>
+    <t>45.98878926437003, 10.35942712940577</t>
+  </si>
+  <si>
+    <t>45.86610443710225, 10.87754308807511</t>
+  </si>
+  <si>
+    <t>45.7691631277102, 12.46473014209328</t>
+  </si>
+  <si>
+    <t>45.65534956312828, 10.15336385115774</t>
+  </si>
+  <si>
+    <t>45.64957308990955, 11.43867283518584</t>
+  </si>
+  <si>
+    <t>46.07574595402827, 9.58046329340464</t>
+  </si>
+  <si>
+    <t>45.67103052766305, 12.101958019341</t>
+  </si>
+  <si>
+    <t>46.1056762133404, 10.77596294598521</t>
+  </si>
+  <si>
+    <t>45.92384945296807, 11.01606710780807</t>
+  </si>
+  <si>
+    <t>45.85198961996426, 11.35797956519265</t>
+  </si>
+  <si>
+    <t>46.05179884948443, 9.9355635516201</t>
+  </si>
+  <si>
+    <t>46.15309688593919, 11.77800541085605</t>
+  </si>
+  <si>
+    <t>46.13082863079344, 9.53854400628652</t>
+  </si>
+  <si>
+    <t>45.64354654319443, 11.88492479025966</t>
+  </si>
+  <si>
+    <t>46.10550779387763, 11.56930069944777</t>
+  </si>
+  <si>
+    <t>45.99844569081272, 11.22187073629392</t>
+  </si>
+  <si>
+    <t>45.43052027945066, 9.5132610624996</t>
+  </si>
+  <si>
+    <t>45.53744566165695, 9.5242329632462</t>
+  </si>
+  <si>
+    <t>45.51574886659327, 10.24511680928524</t>
+  </si>
+  <si>
+    <t>45.70173540865018, 9.95046714981079</t>
+  </si>
+  <si>
+    <t>45.67992301144835, 11.09117581237149</t>
+  </si>
+  <si>
+    <t>45.87985354482004, 11.32176724300472</t>
+  </si>
+  <si>
+    <t>45.49237863467497, 12.23032083541503</t>
+  </si>
+  <si>
+    <t>45.78550790300331, 11.76480985424122</t>
+  </si>
+  <si>
+    <t>45.48338923687622, 11.134756397514</t>
+  </si>
+  <si>
+    <t>45.65678554189262, 11.4489694413703</t>
   </si>
 </sst>
 </file>
@@ -2709,15 +3243,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9737D675-5696-974F-957C-7079EC20390E}">
-  <dimension ref="A1:AJ88"/>
+  <dimension ref="A1:AJ138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+    <sheetView tabSelected="1" topLeftCell="G87" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AE89" sqref="AE89:AE138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.19921875" style="65"/>
+    <col min="3" max="3" width="31.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" style="65" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.09765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="44.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="66" x14ac:dyDescent="0.3">
@@ -2830,7 +3371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -12064,6 +12605,2656 @@
       <c r="AI88" s="58"/>
       <c r="AJ88" s="61"/>
     </row>
+    <row r="89" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>609</v>
+      </c>
+      <c r="B89" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" t="s">
+        <v>610</v>
+      </c>
+      <c r="D89" s="65">
+        <v>38418</v>
+      </c>
+      <c r="E89" t="s">
+        <v>611</v>
+      </c>
+      <c r="G89" t="s">
+        <v>4</v>
+      </c>
+      <c r="J89" t="s">
+        <v>12</v>
+      </c>
+      <c r="K89" s="65">
+        <v>43055</v>
+      </c>
+      <c r="L89" t="s">
+        <v>611</v>
+      </c>
+      <c r="M89" s="65">
+        <v>43989</v>
+      </c>
+      <c r="N89" t="s">
+        <v>611</v>
+      </c>
+      <c r="S89" t="s">
+        <v>63</v>
+      </c>
+      <c r="T89" t="s">
+        <v>14</v>
+      </c>
+      <c r="U89" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y89" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB89" t="s">
+        <v>701</v>
+      </c>
+      <c r="AE89" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="90" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>612</v>
+      </c>
+      <c r="B90" t="s">
+        <v>81</v>
+      </c>
+      <c r="C90" t="s">
+        <v>610</v>
+      </c>
+      <c r="D90" s="65">
+        <v>44157</v>
+      </c>
+      <c r="E90" t="s">
+        <v>613</v>
+      </c>
+      <c r="G90" t="s">
+        <v>4</v>
+      </c>
+      <c r="J90" t="s">
+        <v>611</v>
+      </c>
+      <c r="K90" s="65">
+        <v>41385</v>
+      </c>
+      <c r="L90" t="s">
+        <v>611</v>
+      </c>
+      <c r="M90" s="65">
+        <v>41162</v>
+      </c>
+      <c r="N90">
+        <v>98619</v>
+      </c>
+      <c r="S90" t="s">
+        <v>13</v>
+      </c>
+      <c r="T90" t="s">
+        <v>14</v>
+      </c>
+      <c r="U90" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y90" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB90" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE90" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="91" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>614</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>615</v>
+      </c>
+      <c r="D91" s="65">
+        <v>42369</v>
+      </c>
+      <c r="E91" t="s">
+        <v>613</v>
+      </c>
+      <c r="G91" t="s">
+        <v>4</v>
+      </c>
+      <c r="J91" t="s">
+        <v>611</v>
+      </c>
+      <c r="K91" s="65">
+        <v>40073</v>
+      </c>
+      <c r="L91" t="s">
+        <v>670</v>
+      </c>
+      <c r="M91" s="65">
+        <v>42765</v>
+      </c>
+      <c r="N91">
+        <v>98388</v>
+      </c>
+      <c r="S91" t="s">
+        <v>36</v>
+      </c>
+      <c r="T91" t="s">
+        <v>696</v>
+      </c>
+      <c r="U91" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB91" t="s">
+        <v>702</v>
+      </c>
+      <c r="AE91" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="92" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>616</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>615</v>
+      </c>
+      <c r="D92" s="65">
+        <v>40062</v>
+      </c>
+      <c r="E92" t="s">
+        <v>611</v>
+      </c>
+      <c r="G92" t="s">
+        <v>4</v>
+      </c>
+      <c r="J92" t="s">
+        <v>611</v>
+      </c>
+      <c r="K92" s="65">
+        <v>40483</v>
+      </c>
+      <c r="L92" t="s">
+        <v>611</v>
+      </c>
+      <c r="M92" s="65">
+        <v>42504</v>
+      </c>
+      <c r="N92" t="s">
+        <v>611</v>
+      </c>
+      <c r="S92" t="s">
+        <v>63</v>
+      </c>
+      <c r="T92" t="s">
+        <v>14</v>
+      </c>
+      <c r="U92" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB92" t="s">
+        <v>703</v>
+      </c>
+      <c r="AE92" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="93" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>617</v>
+      </c>
+      <c r="B93" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" t="s">
+        <v>618</v>
+      </c>
+      <c r="D93" s="65">
+        <v>42627</v>
+      </c>
+      <c r="E93" t="s">
+        <v>613</v>
+      </c>
+      <c r="G93" t="s">
+        <v>4</v>
+      </c>
+      <c r="J93" t="s">
+        <v>611</v>
+      </c>
+      <c r="K93" s="65">
+        <v>43816</v>
+      </c>
+      <c r="L93" t="s">
+        <v>671</v>
+      </c>
+      <c r="M93" s="65">
+        <v>41857</v>
+      </c>
+      <c r="N93" t="s">
+        <v>695</v>
+      </c>
+      <c r="S93" t="s">
+        <v>51</v>
+      </c>
+      <c r="T93" t="s">
+        <v>52</v>
+      </c>
+      <c r="U93" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y93" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB93" t="s">
+        <v>704</v>
+      </c>
+      <c r="AE93" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="94" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>619</v>
+      </c>
+      <c r="B94" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" t="s">
+        <v>610</v>
+      </c>
+      <c r="D94" s="65">
+        <v>38454</v>
+      </c>
+      <c r="E94" t="s">
+        <v>611</v>
+      </c>
+      <c r="G94" t="s">
+        <v>4</v>
+      </c>
+      <c r="J94" t="s">
+        <v>611</v>
+      </c>
+      <c r="K94" s="65">
+        <v>40735</v>
+      </c>
+      <c r="L94" t="s">
+        <v>611</v>
+      </c>
+      <c r="M94" s="65">
+        <v>43488</v>
+      </c>
+      <c r="N94">
+        <v>93552</v>
+      </c>
+      <c r="S94" t="s">
+        <v>13</v>
+      </c>
+      <c r="T94" t="s">
+        <v>14</v>
+      </c>
+      <c r="U94" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y94" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB94" t="s">
+        <v>705</v>
+      </c>
+      <c r="AE94" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="95" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>620</v>
+      </c>
+      <c r="B95" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" t="s">
+        <v>610</v>
+      </c>
+      <c r="D95" s="65">
+        <v>43818</v>
+      </c>
+      <c r="E95" t="s">
+        <v>613</v>
+      </c>
+      <c r="G95" t="s">
+        <v>4</v>
+      </c>
+      <c r="J95" t="s">
+        <v>12</v>
+      </c>
+      <c r="K95" s="65">
+        <v>41023</v>
+      </c>
+      <c r="L95" t="s">
+        <v>672</v>
+      </c>
+      <c r="M95" s="65">
+        <v>41058</v>
+      </c>
+      <c r="N95" t="s">
+        <v>611</v>
+      </c>
+      <c r="S95" t="s">
+        <v>51</v>
+      </c>
+      <c r="T95" t="s">
+        <v>52</v>
+      </c>
+      <c r="U95" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y95" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB95" t="s">
+        <v>706</v>
+      </c>
+      <c r="AE95" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="96" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>621</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>615</v>
+      </c>
+      <c r="D96" s="65">
+        <v>40015</v>
+      </c>
+      <c r="E96" t="s">
+        <v>622</v>
+      </c>
+      <c r="G96" t="s">
+        <v>4</v>
+      </c>
+      <c r="J96" t="s">
+        <v>12</v>
+      </c>
+      <c r="K96" s="65">
+        <v>39921</v>
+      </c>
+      <c r="L96" t="s">
+        <v>611</v>
+      </c>
+      <c r="M96" s="65">
+        <v>42407</v>
+      </c>
+      <c r="N96" t="s">
+        <v>611</v>
+      </c>
+      <c r="S96" t="s">
+        <v>22</v>
+      </c>
+      <c r="T96" t="s">
+        <v>14</v>
+      </c>
+      <c r="U96" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y96" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB96" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE96" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="97" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>623</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" t="s">
+        <v>624</v>
+      </c>
+      <c r="D97" s="65">
+        <v>44270</v>
+      </c>
+      <c r="E97" t="s">
+        <v>611</v>
+      </c>
+      <c r="G97" t="s">
+        <v>4</v>
+      </c>
+      <c r="J97" t="s">
+        <v>669</v>
+      </c>
+      <c r="K97" s="65">
+        <v>42604</v>
+      </c>
+      <c r="L97" t="s">
+        <v>673</v>
+      </c>
+      <c r="M97" s="65">
+        <v>41289</v>
+      </c>
+      <c r="N97" t="s">
+        <v>611</v>
+      </c>
+      <c r="S97" t="s">
+        <v>51</v>
+      </c>
+      <c r="T97" t="s">
+        <v>52</v>
+      </c>
+      <c r="U97" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y97" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB97" t="s">
+        <v>707</v>
+      </c>
+      <c r="AE97" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="98" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>625</v>
+      </c>
+      <c r="B98" t="s">
+        <v>61</v>
+      </c>
+      <c r="C98" t="s">
+        <v>626</v>
+      </c>
+      <c r="D98" s="65">
+        <v>43210</v>
+      </c>
+      <c r="E98" t="s">
+        <v>611</v>
+      </c>
+      <c r="G98" t="s">
+        <v>4</v>
+      </c>
+      <c r="J98" t="s">
+        <v>669</v>
+      </c>
+      <c r="K98" s="65">
+        <v>39234</v>
+      </c>
+      <c r="L98" t="s">
+        <v>611</v>
+      </c>
+      <c r="M98" s="65">
+        <v>43296</v>
+      </c>
+      <c r="N98" t="s">
+        <v>695</v>
+      </c>
+      <c r="S98" t="s">
+        <v>13</v>
+      </c>
+      <c r="T98" t="s">
+        <v>14</v>
+      </c>
+      <c r="U98" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y98" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB98" t="s">
+        <v>708</v>
+      </c>
+      <c r="AE98" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="99" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>627</v>
+      </c>
+      <c r="B99" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" t="s">
+        <v>624</v>
+      </c>
+      <c r="D99" s="65">
+        <v>38668</v>
+      </c>
+      <c r="E99" t="s">
+        <v>611</v>
+      </c>
+      <c r="G99" t="s">
+        <v>4</v>
+      </c>
+      <c r="J99" t="s">
+        <v>12</v>
+      </c>
+      <c r="K99" s="65">
+        <v>41137</v>
+      </c>
+      <c r="L99" t="s">
+        <v>611</v>
+      </c>
+      <c r="M99" s="65">
+        <v>41981</v>
+      </c>
+      <c r="N99" t="s">
+        <v>611</v>
+      </c>
+      <c r="S99" t="s">
+        <v>36</v>
+      </c>
+      <c r="T99" t="s">
+        <v>696</v>
+      </c>
+      <c r="U99" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y99" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB99" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE99" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="100" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>628</v>
+      </c>
+      <c r="B100" t="s">
+        <v>31</v>
+      </c>
+      <c r="C100" t="s">
+        <v>629</v>
+      </c>
+      <c r="D100" s="65">
+        <v>42936</v>
+      </c>
+      <c r="E100" t="s">
+        <v>569</v>
+      </c>
+      <c r="G100" t="s">
+        <v>4</v>
+      </c>
+      <c r="J100" t="s">
+        <v>669</v>
+      </c>
+      <c r="K100" s="65">
+        <v>40496</v>
+      </c>
+      <c r="L100" t="s">
+        <v>611</v>
+      </c>
+      <c r="M100" s="65">
+        <v>43506</v>
+      </c>
+      <c r="N100" t="s">
+        <v>695</v>
+      </c>
+      <c r="S100" t="s">
+        <v>63</v>
+      </c>
+      <c r="T100" t="s">
+        <v>14</v>
+      </c>
+      <c r="U100" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y100" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>709</v>
+      </c>
+      <c r="AE100" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="101" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>630</v>
+      </c>
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" t="s">
+        <v>624</v>
+      </c>
+      <c r="D101" s="65">
+        <v>41767</v>
+      </c>
+      <c r="E101" t="s">
+        <v>613</v>
+      </c>
+      <c r="G101" t="s">
+        <v>4</v>
+      </c>
+      <c r="J101" t="s">
+        <v>669</v>
+      </c>
+      <c r="K101" s="65">
+        <v>41126</v>
+      </c>
+      <c r="L101" t="s">
+        <v>611</v>
+      </c>
+      <c r="M101" s="65">
+        <v>40204</v>
+      </c>
+      <c r="N101" t="s">
+        <v>695</v>
+      </c>
+      <c r="S101" t="s">
+        <v>51</v>
+      </c>
+      <c r="T101" t="s">
+        <v>52</v>
+      </c>
+      <c r="U101" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y101" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB101" t="s">
+        <v>710</v>
+      </c>
+      <c r="AE101" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="102" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>631</v>
+      </c>
+      <c r="B102" t="s">
+        <v>81</v>
+      </c>
+      <c r="C102" t="s">
+        <v>610</v>
+      </c>
+      <c r="D102" s="65">
+        <v>39243</v>
+      </c>
+      <c r="E102" t="s">
+        <v>611</v>
+      </c>
+      <c r="G102" t="s">
+        <v>4</v>
+      </c>
+      <c r="J102" t="s">
+        <v>611</v>
+      </c>
+      <c r="K102" s="65">
+        <v>42243</v>
+      </c>
+      <c r="L102" t="s">
+        <v>611</v>
+      </c>
+      <c r="M102" s="65">
+        <v>40866</v>
+      </c>
+      <c r="N102">
+        <v>93477</v>
+      </c>
+      <c r="S102" t="s">
+        <v>63</v>
+      </c>
+      <c r="T102" t="s">
+        <v>14</v>
+      </c>
+      <c r="U102" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y102" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB102" t="s">
+        <v>711</v>
+      </c>
+      <c r="AE102" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="103" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>632</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>615</v>
+      </c>
+      <c r="D103" s="65">
+        <v>40720</v>
+      </c>
+      <c r="E103" t="s">
+        <v>622</v>
+      </c>
+      <c r="G103" t="s">
+        <v>4</v>
+      </c>
+      <c r="J103" t="s">
+        <v>12</v>
+      </c>
+      <c r="K103" s="65">
+        <v>40031</v>
+      </c>
+      <c r="L103" t="s">
+        <v>674</v>
+      </c>
+      <c r="M103" s="65">
+        <v>42451</v>
+      </c>
+      <c r="N103">
+        <v>90003</v>
+      </c>
+      <c r="S103" t="s">
+        <v>22</v>
+      </c>
+      <c r="T103" t="s">
+        <v>14</v>
+      </c>
+      <c r="U103" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y103" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB103" t="s">
+        <v>712</v>
+      </c>
+      <c r="AE103" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="104" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>633</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>615</v>
+      </c>
+      <c r="D104" s="65">
+        <v>43644</v>
+      </c>
+      <c r="E104" t="s">
+        <v>611</v>
+      </c>
+      <c r="G104" t="s">
+        <v>4</v>
+      </c>
+      <c r="J104" t="s">
+        <v>669</v>
+      </c>
+      <c r="K104" s="65">
+        <v>38559</v>
+      </c>
+      <c r="L104" t="s">
+        <v>675</v>
+      </c>
+      <c r="M104" s="65">
+        <v>40186</v>
+      </c>
+      <c r="N104">
+        <v>92705</v>
+      </c>
+      <c r="S104" t="s">
+        <v>36</v>
+      </c>
+      <c r="T104" t="s">
+        <v>696</v>
+      </c>
+      <c r="U104" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y104" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB104" t="s">
+        <v>713</v>
+      </c>
+      <c r="AE104" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="105" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>634</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" t="s">
+        <v>624</v>
+      </c>
+      <c r="D105" s="65">
+        <v>39907</v>
+      </c>
+      <c r="E105" t="s">
+        <v>611</v>
+      </c>
+      <c r="G105" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" t="s">
+        <v>611</v>
+      </c>
+      <c r="K105" s="65">
+        <v>40082</v>
+      </c>
+      <c r="L105" t="s">
+        <v>676</v>
+      </c>
+      <c r="M105" s="65">
+        <v>40629</v>
+      </c>
+      <c r="N105">
+        <v>97419</v>
+      </c>
+      <c r="S105" t="s">
+        <v>63</v>
+      </c>
+      <c r="T105" t="s">
+        <v>14</v>
+      </c>
+      <c r="U105" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y105" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB105" t="s">
+        <v>714</v>
+      </c>
+      <c r="AE105" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="106" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>635</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" t="s">
+        <v>624</v>
+      </c>
+      <c r="D106" s="65">
+        <v>42897</v>
+      </c>
+      <c r="E106" t="s">
+        <v>611</v>
+      </c>
+      <c r="G106" t="s">
+        <v>4</v>
+      </c>
+      <c r="J106" t="s">
+        <v>611</v>
+      </c>
+      <c r="K106" s="65">
+        <v>40369</v>
+      </c>
+      <c r="L106" t="s">
+        <v>677</v>
+      </c>
+      <c r="M106" s="65">
+        <v>42695</v>
+      </c>
+      <c r="N106" t="s">
+        <v>611</v>
+      </c>
+      <c r="S106" t="s">
+        <v>36</v>
+      </c>
+      <c r="T106" t="s">
+        <v>696</v>
+      </c>
+      <c r="U106" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y106" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB106" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE106" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="107" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>636</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>615</v>
+      </c>
+      <c r="D107" s="65">
+        <v>39769</v>
+      </c>
+      <c r="E107" t="s">
+        <v>569</v>
+      </c>
+      <c r="G107" t="s">
+        <v>4</v>
+      </c>
+      <c r="J107" t="s">
+        <v>669</v>
+      </c>
+      <c r="K107" s="65">
+        <v>43346</v>
+      </c>
+      <c r="L107" t="s">
+        <v>678</v>
+      </c>
+      <c r="M107" s="65">
+        <v>42297</v>
+      </c>
+      <c r="N107" t="s">
+        <v>611</v>
+      </c>
+      <c r="S107" t="s">
+        <v>13</v>
+      </c>
+      <c r="T107" t="s">
+        <v>14</v>
+      </c>
+      <c r="U107" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y107" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB107" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE107" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="108" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>637</v>
+      </c>
+      <c r="B108" t="s">
+        <v>46</v>
+      </c>
+      <c r="C108" t="s">
+        <v>638</v>
+      </c>
+      <c r="D108" s="65">
+        <v>43239</v>
+      </c>
+      <c r="E108" t="s">
+        <v>569</v>
+      </c>
+      <c r="G108" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" t="s">
+        <v>12</v>
+      </c>
+      <c r="K108" s="65">
+        <v>39141</v>
+      </c>
+      <c r="L108" t="s">
+        <v>679</v>
+      </c>
+      <c r="M108" s="65">
+        <v>44386</v>
+      </c>
+      <c r="N108">
+        <v>94679</v>
+      </c>
+      <c r="S108" t="s">
+        <v>13</v>
+      </c>
+      <c r="T108" t="s">
+        <v>14</v>
+      </c>
+      <c r="U108" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y108" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB108" t="s">
+        <v>715</v>
+      </c>
+      <c r="AE108" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="109" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>639</v>
+      </c>
+      <c r="B109" t="s">
+        <v>46</v>
+      </c>
+      <c r="C109" t="s">
+        <v>638</v>
+      </c>
+      <c r="D109" s="65">
+        <v>43915</v>
+      </c>
+      <c r="E109" t="s">
+        <v>613</v>
+      </c>
+      <c r="G109" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" t="s">
+        <v>12</v>
+      </c>
+      <c r="K109" s="65">
+        <v>42918</v>
+      </c>
+      <c r="L109" t="s">
+        <v>611</v>
+      </c>
+      <c r="M109" s="65">
+        <v>41022</v>
+      </c>
+      <c r="N109" t="s">
+        <v>611</v>
+      </c>
+      <c r="S109" t="s">
+        <v>13</v>
+      </c>
+      <c r="T109" t="s">
+        <v>14</v>
+      </c>
+      <c r="U109" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y109" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB109" t="s">
+        <v>716</v>
+      </c>
+      <c r="AE109" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="110" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>640</v>
+      </c>
+      <c r="B110" t="s">
+        <v>61</v>
+      </c>
+      <c r="C110" t="s">
+        <v>626</v>
+      </c>
+      <c r="D110" s="65">
+        <v>42099</v>
+      </c>
+      <c r="E110" t="s">
+        <v>622</v>
+      </c>
+      <c r="G110" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" t="s">
+        <v>669</v>
+      </c>
+      <c r="K110" s="65">
+        <v>39157</v>
+      </c>
+      <c r="L110" t="s">
+        <v>611</v>
+      </c>
+      <c r="M110" s="65">
+        <v>41544</v>
+      </c>
+      <c r="N110" t="s">
+        <v>611</v>
+      </c>
+      <c r="S110" t="s">
+        <v>51</v>
+      </c>
+      <c r="T110" t="s">
+        <v>52</v>
+      </c>
+      <c r="U110" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y110" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB110" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE110" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="111" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>641</v>
+      </c>
+      <c r="B111" t="s">
+        <v>31</v>
+      </c>
+      <c r="C111" t="s">
+        <v>629</v>
+      </c>
+      <c r="D111" s="65">
+        <v>41197</v>
+      </c>
+      <c r="E111" t="s">
+        <v>622</v>
+      </c>
+      <c r="G111" t="s">
+        <v>4</v>
+      </c>
+      <c r="J111" t="s">
+        <v>669</v>
+      </c>
+      <c r="K111" s="65">
+        <v>38705</v>
+      </c>
+      <c r="L111" t="s">
+        <v>680</v>
+      </c>
+      <c r="M111" s="65">
+        <v>40577</v>
+      </c>
+      <c r="N111" t="s">
+        <v>695</v>
+      </c>
+      <c r="S111" t="s">
+        <v>22</v>
+      </c>
+      <c r="T111" t="s">
+        <v>14</v>
+      </c>
+      <c r="U111" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y111" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB111" t="s">
+        <v>717</v>
+      </c>
+      <c r="AE111" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="112" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>642</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>615</v>
+      </c>
+      <c r="D112" s="65">
+        <v>43143</v>
+      </c>
+      <c r="E112" t="s">
+        <v>622</v>
+      </c>
+      <c r="G112" t="s">
+        <v>4</v>
+      </c>
+      <c r="J112" t="s">
+        <v>611</v>
+      </c>
+      <c r="K112" s="65">
+        <v>38615</v>
+      </c>
+      <c r="L112" t="s">
+        <v>681</v>
+      </c>
+      <c r="M112" s="65">
+        <v>41965</v>
+      </c>
+      <c r="N112">
+        <v>98117</v>
+      </c>
+      <c r="S112" t="s">
+        <v>36</v>
+      </c>
+      <c r="T112" t="s">
+        <v>696</v>
+      </c>
+      <c r="U112" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y112" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB112" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE112" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="113" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>643</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>615</v>
+      </c>
+      <c r="D113" s="65">
+        <v>40688</v>
+      </c>
+      <c r="E113" t="s">
+        <v>613</v>
+      </c>
+      <c r="G113" t="s">
+        <v>4</v>
+      </c>
+      <c r="J113" t="s">
+        <v>669</v>
+      </c>
+      <c r="K113" s="65">
+        <v>40503</v>
+      </c>
+      <c r="L113" t="s">
+        <v>611</v>
+      </c>
+      <c r="M113" s="65">
+        <v>43773</v>
+      </c>
+      <c r="N113">
+        <v>93528</v>
+      </c>
+      <c r="S113" t="s">
+        <v>36</v>
+      </c>
+      <c r="T113" t="s">
+        <v>696</v>
+      </c>
+      <c r="U113" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y113" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB113" t="s">
+        <v>718</v>
+      </c>
+      <c r="AE113" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="114" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>644</v>
+      </c>
+      <c r="B114" t="s">
+        <v>81</v>
+      </c>
+      <c r="C114" t="s">
+        <v>610</v>
+      </c>
+      <c r="D114" s="65">
+        <v>39264</v>
+      </c>
+      <c r="E114" t="s">
+        <v>613</v>
+      </c>
+      <c r="G114" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" t="s">
+        <v>611</v>
+      </c>
+      <c r="K114" s="65">
+        <v>39457</v>
+      </c>
+      <c r="L114" t="s">
+        <v>611</v>
+      </c>
+      <c r="M114" s="65">
+        <v>42402</v>
+      </c>
+      <c r="N114">
+        <v>95774</v>
+      </c>
+      <c r="S114" t="s">
+        <v>22</v>
+      </c>
+      <c r="T114" t="s">
+        <v>14</v>
+      </c>
+      <c r="U114" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y114" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB114" t="s">
+        <v>719</v>
+      </c>
+      <c r="AE114" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="115" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>645</v>
+      </c>
+      <c r="B115" t="s">
+        <v>61</v>
+      </c>
+      <c r="C115" t="s">
+        <v>626</v>
+      </c>
+      <c r="D115" s="65">
+        <v>38585</v>
+      </c>
+      <c r="E115" t="s">
+        <v>611</v>
+      </c>
+      <c r="G115" t="s">
+        <v>4</v>
+      </c>
+      <c r="J115" t="s">
+        <v>669</v>
+      </c>
+      <c r="K115" s="65">
+        <v>39212</v>
+      </c>
+      <c r="L115" t="s">
+        <v>682</v>
+      </c>
+      <c r="M115" s="65">
+        <v>42850</v>
+      </c>
+      <c r="N115" t="s">
+        <v>611</v>
+      </c>
+      <c r="S115" t="s">
+        <v>51</v>
+      </c>
+      <c r="T115" t="s">
+        <v>52</v>
+      </c>
+      <c r="U115" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y115" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB115" t="s">
+        <v>720</v>
+      </c>
+      <c r="AE115" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="116" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>646</v>
+      </c>
+      <c r="B116" t="s">
+        <v>46</v>
+      </c>
+      <c r="C116" t="s">
+        <v>638</v>
+      </c>
+      <c r="D116" s="65">
+        <v>43992</v>
+      </c>
+      <c r="E116" t="s">
+        <v>569</v>
+      </c>
+      <c r="G116" t="s">
+        <v>4</v>
+      </c>
+      <c r="J116" t="s">
+        <v>669</v>
+      </c>
+      <c r="K116" s="65">
+        <v>39318</v>
+      </c>
+      <c r="L116" t="s">
+        <v>683</v>
+      </c>
+      <c r="M116" s="65">
+        <v>44680</v>
+      </c>
+      <c r="N116" t="s">
+        <v>611</v>
+      </c>
+      <c r="S116" t="s">
+        <v>22</v>
+      </c>
+      <c r="T116" t="s">
+        <v>14</v>
+      </c>
+      <c r="U116" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y116" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB116" t="s">
+        <v>721</v>
+      </c>
+      <c r="AE116" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="117" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>647</v>
+      </c>
+      <c r="B117" t="s">
+        <v>71</v>
+      </c>
+      <c r="C117" t="s">
+        <v>618</v>
+      </c>
+      <c r="D117" s="65">
+        <v>43250</v>
+      </c>
+      <c r="E117" t="s">
+        <v>613</v>
+      </c>
+      <c r="G117" t="s">
+        <v>4</v>
+      </c>
+      <c r="J117" t="s">
+        <v>12</v>
+      </c>
+      <c r="K117" s="65">
+        <v>40939</v>
+      </c>
+      <c r="L117" t="s">
+        <v>684</v>
+      </c>
+      <c r="M117" s="65">
+        <v>40298</v>
+      </c>
+      <c r="N117">
+        <v>99514</v>
+      </c>
+      <c r="S117" t="s">
+        <v>51</v>
+      </c>
+      <c r="T117" t="s">
+        <v>52</v>
+      </c>
+      <c r="U117" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y117" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB117" t="s">
+        <v>722</v>
+      </c>
+      <c r="AE117" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="118" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>648</v>
+      </c>
+      <c r="B118" t="s">
+        <v>31</v>
+      </c>
+      <c r="C118" t="s">
+        <v>629</v>
+      </c>
+      <c r="D118" s="65">
+        <v>42863</v>
+      </c>
+      <c r="E118" t="s">
+        <v>611</v>
+      </c>
+      <c r="G118" t="s">
+        <v>4</v>
+      </c>
+      <c r="J118" t="s">
+        <v>12</v>
+      </c>
+      <c r="K118" s="65">
+        <v>42920</v>
+      </c>
+      <c r="L118" t="s">
+        <v>611</v>
+      </c>
+      <c r="M118" s="65">
+        <v>41057</v>
+      </c>
+      <c r="N118">
+        <v>99134</v>
+      </c>
+      <c r="S118" t="s">
+        <v>13</v>
+      </c>
+      <c r="T118" t="s">
+        <v>14</v>
+      </c>
+      <c r="U118" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y118" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB118" t="s">
+        <v>723</v>
+      </c>
+      <c r="AE118" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="119" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>649</v>
+      </c>
+      <c r="B119" t="s">
+        <v>31</v>
+      </c>
+      <c r="C119" t="s">
+        <v>629</v>
+      </c>
+      <c r="D119" s="65">
+        <v>40953</v>
+      </c>
+      <c r="E119" t="s">
+        <v>622</v>
+      </c>
+      <c r="G119" t="s">
+        <v>4</v>
+      </c>
+      <c r="J119" t="s">
+        <v>12</v>
+      </c>
+      <c r="K119" s="65">
+        <v>42327</v>
+      </c>
+      <c r="L119" t="s">
+        <v>611</v>
+      </c>
+      <c r="M119" s="65">
+        <v>41616</v>
+      </c>
+      <c r="N119" t="s">
+        <v>695</v>
+      </c>
+      <c r="S119" t="s">
+        <v>63</v>
+      </c>
+      <c r="T119" t="s">
+        <v>14</v>
+      </c>
+      <c r="U119" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y119" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB119" t="s">
+        <v>724</v>
+      </c>
+      <c r="AE119" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="120" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>650</v>
+      </c>
+      <c r="B120" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120" t="s">
+        <v>629</v>
+      </c>
+      <c r="D120" s="65">
+        <v>42598</v>
+      </c>
+      <c r="E120" t="s">
+        <v>613</v>
+      </c>
+      <c r="G120" t="s">
+        <v>4</v>
+      </c>
+      <c r="J120" t="s">
+        <v>12</v>
+      </c>
+      <c r="K120" s="65">
+        <v>42145</v>
+      </c>
+      <c r="L120" t="s">
+        <v>685</v>
+      </c>
+      <c r="M120" s="65">
+        <v>43277</v>
+      </c>
+      <c r="N120" t="s">
+        <v>611</v>
+      </c>
+      <c r="S120" t="s">
+        <v>51</v>
+      </c>
+      <c r="T120" t="s">
+        <v>52</v>
+      </c>
+      <c r="U120" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y120" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB120" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE120" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="121" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>651</v>
+      </c>
+      <c r="B121" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" t="s">
+        <v>624</v>
+      </c>
+      <c r="D121" s="65">
+        <v>40371</v>
+      </c>
+      <c r="E121" t="s">
+        <v>611</v>
+      </c>
+      <c r="G121" t="s">
+        <v>4</v>
+      </c>
+      <c r="J121" t="s">
+        <v>611</v>
+      </c>
+      <c r="K121" s="65">
+        <v>42179</v>
+      </c>
+      <c r="L121" t="s">
+        <v>686</v>
+      </c>
+      <c r="M121" s="65">
+        <v>40648</v>
+      </c>
+      <c r="N121" t="s">
+        <v>611</v>
+      </c>
+      <c r="S121" t="s">
+        <v>51</v>
+      </c>
+      <c r="T121" t="s">
+        <v>52</v>
+      </c>
+      <c r="U121" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y121" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB121" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE121" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="122" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>652</v>
+      </c>
+      <c r="B122" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s">
+        <v>624</v>
+      </c>
+      <c r="D122" s="65">
+        <v>41901</v>
+      </c>
+      <c r="E122" t="s">
+        <v>622</v>
+      </c>
+      <c r="G122" t="s">
+        <v>4</v>
+      </c>
+      <c r="J122" t="s">
+        <v>669</v>
+      </c>
+      <c r="K122" s="65">
+        <v>41190</v>
+      </c>
+      <c r="L122" t="s">
+        <v>611</v>
+      </c>
+      <c r="M122" s="65">
+        <v>42574</v>
+      </c>
+      <c r="N122" t="s">
+        <v>611</v>
+      </c>
+      <c r="S122" t="s">
+        <v>13</v>
+      </c>
+      <c r="T122" t="s">
+        <v>14</v>
+      </c>
+      <c r="U122" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y122" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB122" t="s">
+        <v>725</v>
+      </c>
+      <c r="AE122" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="123" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>653</v>
+      </c>
+      <c r="B123" t="s">
+        <v>61</v>
+      </c>
+      <c r="C123" t="s">
+        <v>626</v>
+      </c>
+      <c r="D123" s="65">
+        <v>39542</v>
+      </c>
+      <c r="E123" t="s">
+        <v>569</v>
+      </c>
+      <c r="G123" t="s">
+        <v>4</v>
+      </c>
+      <c r="J123" t="s">
+        <v>12</v>
+      </c>
+      <c r="K123" s="65">
+        <v>43395</v>
+      </c>
+      <c r="L123" t="s">
+        <v>687</v>
+      </c>
+      <c r="M123" s="65">
+        <v>42915</v>
+      </c>
+      <c r="N123" t="s">
+        <v>695</v>
+      </c>
+      <c r="S123" t="s">
+        <v>22</v>
+      </c>
+      <c r="T123" t="s">
+        <v>14</v>
+      </c>
+      <c r="U123" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y123" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB123" t="s">
+        <v>726</v>
+      </c>
+      <c r="AE123" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="124" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>654</v>
+      </c>
+      <c r="B124" t="s">
+        <v>81</v>
+      </c>
+      <c r="C124" t="s">
+        <v>610</v>
+      </c>
+      <c r="D124" s="65">
+        <v>39065</v>
+      </c>
+      <c r="E124" t="s">
+        <v>611</v>
+      </c>
+      <c r="G124" t="s">
+        <v>4</v>
+      </c>
+      <c r="J124" t="s">
+        <v>611</v>
+      </c>
+      <c r="K124" s="65">
+        <v>41566</v>
+      </c>
+      <c r="L124" t="s">
+        <v>611</v>
+      </c>
+      <c r="M124" s="65">
+        <v>43571</v>
+      </c>
+      <c r="N124" t="s">
+        <v>695</v>
+      </c>
+      <c r="S124" t="s">
+        <v>51</v>
+      </c>
+      <c r="T124" t="s">
+        <v>52</v>
+      </c>
+      <c r="U124" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y124" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB124" t="s">
+        <v>727</v>
+      </c>
+      <c r="AE124" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="125" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>655</v>
+      </c>
+      <c r="B125" t="s">
+        <v>46</v>
+      </c>
+      <c r="C125" t="s">
+        <v>638</v>
+      </c>
+      <c r="D125" s="65">
+        <v>41646</v>
+      </c>
+      <c r="E125" t="s">
+        <v>569</v>
+      </c>
+      <c r="G125" t="s">
+        <v>4</v>
+      </c>
+      <c r="J125" t="s">
+        <v>611</v>
+      </c>
+      <c r="K125" s="65">
+        <v>40403</v>
+      </c>
+      <c r="L125" t="s">
+        <v>611</v>
+      </c>
+      <c r="M125" s="65">
+        <v>43161</v>
+      </c>
+      <c r="N125" t="s">
+        <v>695</v>
+      </c>
+      <c r="S125" t="s">
+        <v>51</v>
+      </c>
+      <c r="T125" t="s">
+        <v>52</v>
+      </c>
+      <c r="U125" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y125" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB125" t="s">
+        <v>728</v>
+      </c>
+      <c r="AE125" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="126" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>656</v>
+      </c>
+      <c r="B126" t="s">
+        <v>71</v>
+      </c>
+      <c r="C126" t="s">
+        <v>618</v>
+      </c>
+      <c r="D126" s="65">
+        <v>38447</v>
+      </c>
+      <c r="E126" t="s">
+        <v>569</v>
+      </c>
+      <c r="G126" t="s">
+        <v>4</v>
+      </c>
+      <c r="J126" t="s">
+        <v>12</v>
+      </c>
+      <c r="K126" s="65">
+        <v>43334</v>
+      </c>
+      <c r="L126" t="s">
+        <v>688</v>
+      </c>
+      <c r="M126" s="65">
+        <v>41681</v>
+      </c>
+      <c r="N126" t="s">
+        <v>695</v>
+      </c>
+      <c r="S126" t="s">
+        <v>22</v>
+      </c>
+      <c r="T126" t="s">
+        <v>14</v>
+      </c>
+      <c r="U126" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y126" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB126" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE126" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="127" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>657</v>
+      </c>
+      <c r="B127" t="s">
+        <v>71</v>
+      </c>
+      <c r="C127" t="s">
+        <v>618</v>
+      </c>
+      <c r="D127" s="65">
+        <v>43128</v>
+      </c>
+      <c r="E127" t="s">
+        <v>613</v>
+      </c>
+      <c r="G127" t="s">
+        <v>4</v>
+      </c>
+      <c r="J127" t="s">
+        <v>611</v>
+      </c>
+      <c r="K127" s="65">
+        <v>41853</v>
+      </c>
+      <c r="L127" t="s">
+        <v>611</v>
+      </c>
+      <c r="M127" s="65">
+        <v>42339</v>
+      </c>
+      <c r="N127" t="s">
+        <v>611</v>
+      </c>
+      <c r="S127" t="s">
+        <v>13</v>
+      </c>
+      <c r="T127" t="s">
+        <v>14</v>
+      </c>
+      <c r="U127" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y127" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB127" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE127" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="128" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>658</v>
+      </c>
+      <c r="B128" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128" t="s">
+        <v>624</v>
+      </c>
+      <c r="D128" s="65">
+        <v>44172</v>
+      </c>
+      <c r="E128" t="s">
+        <v>613</v>
+      </c>
+      <c r="G128" t="s">
+        <v>4</v>
+      </c>
+      <c r="J128" t="s">
+        <v>611</v>
+      </c>
+      <c r="K128" s="65">
+        <v>38863</v>
+      </c>
+      <c r="L128" t="s">
+        <v>689</v>
+      </c>
+      <c r="M128" s="65">
+        <v>44077</v>
+      </c>
+      <c r="N128" t="s">
+        <v>611</v>
+      </c>
+      <c r="S128" t="s">
+        <v>36</v>
+      </c>
+      <c r="T128" t="s">
+        <v>696</v>
+      </c>
+      <c r="U128" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y128" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB128" t="s">
+        <v>729</v>
+      </c>
+      <c r="AE128" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="129" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>659</v>
+      </c>
+      <c r="B129" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129" t="s">
+        <v>626</v>
+      </c>
+      <c r="D129" s="65">
+        <v>43499</v>
+      </c>
+      <c r="E129" t="s">
+        <v>622</v>
+      </c>
+      <c r="G129" t="s">
+        <v>4</v>
+      </c>
+      <c r="J129" t="s">
+        <v>12</v>
+      </c>
+      <c r="K129" s="65">
+        <v>42692</v>
+      </c>
+      <c r="L129" t="s">
+        <v>611</v>
+      </c>
+      <c r="M129" s="65">
+        <v>40761</v>
+      </c>
+      <c r="N129" t="s">
+        <v>695</v>
+      </c>
+      <c r="S129" t="s">
+        <v>22</v>
+      </c>
+      <c r="T129" t="s">
+        <v>14</v>
+      </c>
+      <c r="U129" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y129" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB129" t="s">
+        <v>730</v>
+      </c>
+      <c r="AE129" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="130" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>660</v>
+      </c>
+      <c r="B130" t="s">
+        <v>61</v>
+      </c>
+      <c r="C130" t="s">
+        <v>626</v>
+      </c>
+      <c r="D130" s="65">
+        <v>43591</v>
+      </c>
+      <c r="E130" t="s">
+        <v>613</v>
+      </c>
+      <c r="G130" t="s">
+        <v>4</v>
+      </c>
+      <c r="J130" t="s">
+        <v>669</v>
+      </c>
+      <c r="K130" s="65">
+        <v>43667</v>
+      </c>
+      <c r="L130" t="s">
+        <v>690</v>
+      </c>
+      <c r="M130" s="65">
+        <v>40423</v>
+      </c>
+      <c r="N130">
+        <v>95640</v>
+      </c>
+      <c r="S130" t="s">
+        <v>63</v>
+      </c>
+      <c r="T130" t="s">
+        <v>14</v>
+      </c>
+      <c r="U130" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y130" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB130" t="s">
+        <v>731</v>
+      </c>
+      <c r="AE130" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="131" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>661</v>
+      </c>
+      <c r="B131" t="s">
+        <v>31</v>
+      </c>
+      <c r="C131" t="s">
+        <v>629</v>
+      </c>
+      <c r="D131" s="65">
+        <v>44215</v>
+      </c>
+      <c r="E131" t="s">
+        <v>613</v>
+      </c>
+      <c r="G131" t="s">
+        <v>4</v>
+      </c>
+      <c r="J131" t="s">
+        <v>611</v>
+      </c>
+      <c r="K131" s="65">
+        <v>40424</v>
+      </c>
+      <c r="L131" t="s">
+        <v>611</v>
+      </c>
+      <c r="M131" s="65">
+        <v>42523</v>
+      </c>
+      <c r="N131" t="s">
+        <v>611</v>
+      </c>
+      <c r="S131" t="s">
+        <v>13</v>
+      </c>
+      <c r="T131" t="s">
+        <v>14</v>
+      </c>
+      <c r="U131" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y131" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB131" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE131" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="132" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>662</v>
+      </c>
+      <c r="B132" t="s">
+        <v>71</v>
+      </c>
+      <c r="C132" t="s">
+        <v>618</v>
+      </c>
+      <c r="D132" s="65">
+        <v>40848</v>
+      </c>
+      <c r="E132" t="s">
+        <v>569</v>
+      </c>
+      <c r="G132" t="s">
+        <v>4</v>
+      </c>
+      <c r="J132" t="s">
+        <v>669</v>
+      </c>
+      <c r="K132" s="65">
+        <v>43124</v>
+      </c>
+      <c r="L132" t="s">
+        <v>691</v>
+      </c>
+      <c r="M132" s="65">
+        <v>43154</v>
+      </c>
+      <c r="N132">
+        <v>95833</v>
+      </c>
+      <c r="S132" t="s">
+        <v>51</v>
+      </c>
+      <c r="T132" t="s">
+        <v>52</v>
+      </c>
+      <c r="U132" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y132" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB132" t="s">
+        <v>732</v>
+      </c>
+      <c r="AE132" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="133" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>663</v>
+      </c>
+      <c r="B133" t="s">
+        <v>31</v>
+      </c>
+      <c r="C133" t="s">
+        <v>629</v>
+      </c>
+      <c r="D133" s="65">
+        <v>40787</v>
+      </c>
+      <c r="E133" t="s">
+        <v>622</v>
+      </c>
+      <c r="G133" t="s">
+        <v>4</v>
+      </c>
+      <c r="J133" t="s">
+        <v>669</v>
+      </c>
+      <c r="K133" s="65">
+        <v>40587</v>
+      </c>
+      <c r="L133" t="s">
+        <v>692</v>
+      </c>
+      <c r="M133" s="65">
+        <v>42992</v>
+      </c>
+      <c r="N133" t="s">
+        <v>611</v>
+      </c>
+      <c r="S133" t="s">
+        <v>13</v>
+      </c>
+      <c r="T133" t="s">
+        <v>14</v>
+      </c>
+      <c r="U133" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y133" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB133" t="s">
+        <v>733</v>
+      </c>
+      <c r="AE133" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="134" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>664</v>
+      </c>
+      <c r="B134" t="s">
+        <v>46</v>
+      </c>
+      <c r="C134" t="s">
+        <v>638</v>
+      </c>
+      <c r="D134" s="65">
+        <v>40046</v>
+      </c>
+      <c r="E134" t="s">
+        <v>611</v>
+      </c>
+      <c r="G134" t="s">
+        <v>4</v>
+      </c>
+      <c r="J134" t="s">
+        <v>669</v>
+      </c>
+      <c r="K134" s="65">
+        <v>40189</v>
+      </c>
+      <c r="L134" t="s">
+        <v>693</v>
+      </c>
+      <c r="M134" s="65">
+        <v>43019</v>
+      </c>
+      <c r="N134">
+        <v>95420</v>
+      </c>
+      <c r="S134" t="s">
+        <v>51</v>
+      </c>
+      <c r="T134" t="s">
+        <v>52</v>
+      </c>
+      <c r="U134" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y134" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB134" t="s">
+        <v>734</v>
+      </c>
+      <c r="AE134" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="135" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>665</v>
+      </c>
+      <c r="B135" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" t="s">
+        <v>624</v>
+      </c>
+      <c r="D135" s="65">
+        <v>40432</v>
+      </c>
+      <c r="E135" t="s">
+        <v>611</v>
+      </c>
+      <c r="G135" t="s">
+        <v>4</v>
+      </c>
+      <c r="J135" t="s">
+        <v>12</v>
+      </c>
+      <c r="K135" s="65">
+        <v>39575</v>
+      </c>
+      <c r="L135" t="s">
+        <v>611</v>
+      </c>
+      <c r="M135" s="65">
+        <v>43080</v>
+      </c>
+      <c r="N135" t="s">
+        <v>611</v>
+      </c>
+      <c r="S135" t="s">
+        <v>36</v>
+      </c>
+      <c r="T135" t="s">
+        <v>696</v>
+      </c>
+      <c r="U135" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y135" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB135" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE135" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="136" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>666</v>
+      </c>
+      <c r="B136" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" t="s">
+        <v>624</v>
+      </c>
+      <c r="D136" s="65">
+        <v>38965</v>
+      </c>
+      <c r="E136" t="s">
+        <v>622</v>
+      </c>
+      <c r="G136" t="s">
+        <v>4</v>
+      </c>
+      <c r="J136" t="s">
+        <v>12</v>
+      </c>
+      <c r="K136" s="65">
+        <v>43326</v>
+      </c>
+      <c r="L136" t="s">
+        <v>611</v>
+      </c>
+      <c r="M136" s="65">
+        <v>40621</v>
+      </c>
+      <c r="N136" t="s">
+        <v>695</v>
+      </c>
+      <c r="S136" t="s">
+        <v>63</v>
+      </c>
+      <c r="T136" t="s">
+        <v>14</v>
+      </c>
+      <c r="U136" t="s">
+        <v>700</v>
+      </c>
+      <c r="Y136" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB136" t="s">
+        <v>703</v>
+      </c>
+      <c r="AE136" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="137" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>667</v>
+      </c>
+      <c r="B137" t="s">
+        <v>31</v>
+      </c>
+      <c r="C137" t="s">
+        <v>629</v>
+      </c>
+      <c r="D137" s="65">
+        <v>42007</v>
+      </c>
+      <c r="E137" t="s">
+        <v>611</v>
+      </c>
+      <c r="G137" t="s">
+        <v>4</v>
+      </c>
+      <c r="J137" t="s">
+        <v>611</v>
+      </c>
+      <c r="K137" s="65">
+        <v>40393</v>
+      </c>
+      <c r="L137" t="s">
+        <v>694</v>
+      </c>
+      <c r="M137" s="65">
+        <v>42845</v>
+      </c>
+      <c r="N137">
+        <v>93552</v>
+      </c>
+      <c r="S137" t="s">
+        <v>36</v>
+      </c>
+      <c r="T137" t="s">
+        <v>696</v>
+      </c>
+      <c r="U137" t="s">
+        <v>699</v>
+      </c>
+      <c r="Y137" t="s">
+        <v>736</v>
+      </c>
+      <c r="AB137" t="s">
+        <v>735</v>
+      </c>
+      <c r="AE137" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="138" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>668</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
+        <v>615</v>
+      </c>
+      <c r="D138" s="65">
+        <v>39755</v>
+      </c>
+      <c r="E138" t="s">
+        <v>613</v>
+      </c>
+      <c r="G138" t="s">
+        <v>4</v>
+      </c>
+      <c r="J138" t="s">
+        <v>611</v>
+      </c>
+      <c r="K138" s="65">
+        <v>43269</v>
+      </c>
+      <c r="L138" t="s">
+        <v>611</v>
+      </c>
+      <c r="M138" s="65">
+        <v>42267</v>
+      </c>
+      <c r="N138" t="s">
+        <v>611</v>
+      </c>
+      <c r="S138" t="s">
+        <v>13</v>
+      </c>
+      <c r="T138" t="s">
+        <v>14</v>
+      </c>
+      <c r="U138" t="s">
+        <v>611</v>
+      </c>
+      <c r="Y138" t="s">
+        <v>611</v>
+      </c>
+      <c r="AB138" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE138" t="s">
+        <v>786</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>